<commit_message>
table save an prev table
</commit_message>
<xml_diff>
--- a/data/planner.xlsx
+++ b/data/planner.xlsx
@@ -58,11 +58,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -432,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK13"/>
+  <dimension ref="A1:AK14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,160 +439,120 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="n">
-        <v>44927</v>
-      </c>
-      <c r="B1" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>ОШ</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Unnamed: 4</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="n">
-        <v>16449</v>
-      </c>
-      <c r="H1" s="2" t="n">
-        <v>49807</v>
-      </c>
-      <c r="I1" s="2" t="n">
-        <v>34079</v>
-      </c>
-      <c r="J1" s="2" t="n">
-        <v>38885</v>
-      </c>
-      <c r="K1" s="2" t="n">
-        <v>9366</v>
-      </c>
-      <c r="L1" s="2" t="n">
-        <v>9859</v>
-      </c>
-      <c r="M1" s="2" t="n">
-        <v>9746</v>
-      </c>
-      <c r="N1" s="2" t="inlineStr">
-        <is>
-          <t>|.1</t>
-        </is>
-      </c>
-      <c r="O1" s="2" t="n">
-        <v>40651</v>
-      </c>
-      <c r="P1" s="2" t="n">
-        <v>19763</v>
-      </c>
-      <c r="Q1" s="2" t="n">
-        <v>15336</v>
-      </c>
-      <c r="R1" s="2" t="n">
-        <v>58529</v>
-      </c>
-      <c r="S1" s="2" t="n">
-        <v>30309</v>
-      </c>
-      <c r="T1" s="2" t="n">
-        <v>26194</v>
-      </c>
-      <c r="U1" s="2" t="n">
-        <v>8881</v>
-      </c>
-      <c r="V1" s="2" t="inlineStr">
-        <is>
-          <t>|.2</t>
-        </is>
-      </c>
-      <c r="W1" s="2" t="inlineStr">
-        <is>
-          <t>М</t>
-        </is>
-      </c>
-      <c r="X1" s="2" t="inlineStr">
-        <is>
-          <t>М.1</t>
-        </is>
-      </c>
-      <c r="Y1" s="2" t="inlineStr">
-        <is>
-          <t>М.2</t>
-        </is>
-      </c>
-      <c r="Z1" s="2" t="inlineStr">
-        <is>
-          <t>М.3</t>
-        </is>
-      </c>
-      <c r="AA1" s="2" t="inlineStr">
-        <is>
-          <t>М.4</t>
-        </is>
-      </c>
-      <c r="AB1" s="2" t="inlineStr">
-        <is>
-          <t>М.5</t>
-        </is>
-      </c>
-      <c r="AC1" s="2" t="inlineStr">
-        <is>
-          <t>М.6</t>
-        </is>
-      </c>
-      <c r="AD1" s="2" t="inlineStr">
-        <is>
-          <t>Р</t>
-        </is>
-      </c>
-      <c r="AE1" s="2" t="inlineStr">
-        <is>
-          <t>М.7</t>
-        </is>
-      </c>
-      <c r="AF1" s="2" t="inlineStr">
-        <is>
-          <t>М.8</t>
-        </is>
-      </c>
-      <c r="AG1" s="2" t="inlineStr">
-        <is>
-          <t>Р.1</t>
-        </is>
-      </c>
-      <c r="AH1" s="2" t="inlineStr">
-        <is>
-          <t>Р.2</t>
-        </is>
-      </c>
-      <c r="AI1" s="2" t="inlineStr">
-        <is>
-          <t>ПР</t>
-        </is>
-      </c>
-      <c r="AJ1" s="2" t="inlineStr">
-        <is>
-          <t>М.9</t>
-        </is>
-      </c>
-      <c r="AK1" s="2" t="inlineStr">
-        <is>
-          <t>М.10</t>
-        </is>
+      <c r="F1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="n">
-        <v>44928</v>
+      <c r="A2" s="2" t="n">
+        <v>44927</v>
       </c>
       <c r="B2" t="n">
         <v>5</v>
@@ -615,25 +572,25 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>16473</v>
+        <v>1111</v>
       </c>
       <c r="H2" t="n">
-        <v>49831</v>
+        <v>49807</v>
       </c>
       <c r="I2" t="n">
-        <v>34103</v>
+        <v>34079</v>
       </c>
       <c r="J2" t="n">
-        <v>38909</v>
+        <v>38885</v>
       </c>
       <c r="K2" t="n">
-        <v>9390</v>
+        <v>9366</v>
       </c>
       <c r="L2" t="n">
-        <v>9883</v>
+        <v>9859</v>
       </c>
       <c r="M2" t="n">
-        <v>9770</v>
+        <v>9746</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -641,10 +598,10 @@
         </is>
       </c>
       <c r="O2" t="n">
-        <v>40675</v>
+        <v>40651</v>
       </c>
       <c r="P2" t="n">
-        <v>19787</v>
+        <v>19763</v>
       </c>
       <c r="Q2" t="n">
         <v>15336</v>
@@ -656,10 +613,10 @@
         <v>30309</v>
       </c>
       <c r="T2" t="n">
-        <v>26218</v>
+        <v>26194</v>
       </c>
       <c r="U2" t="n">
-        <v>8905</v>
+        <v>8881</v>
       </c>
       <c r="V2" t="inlineStr">
         <is>
@@ -718,17 +675,17 @@
       </c>
       <c r="AG2" t="inlineStr">
         <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
           <t>ПР</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>Р</t>
-        </is>
-      </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>Р</t>
         </is>
       </c>
       <c r="AJ2" t="inlineStr">
@@ -743,8 +700,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="n">
-        <v>44929</v>
+      <c r="A3" s="2" t="n">
+        <v>44928</v>
       </c>
       <c r="B3" t="n">
         <v>5</v>
@@ -752,7 +709,11 @@
       <c r="C3" t="n">
         <v>4</v>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ОШ</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
@@ -760,25 +721,25 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>16473</v>
+        <v>2222</v>
       </c>
       <c r="H3" t="n">
-        <v>49855</v>
+        <v>49831</v>
       </c>
       <c r="I3" t="n">
         <v>34103</v>
       </c>
       <c r="J3" t="n">
-        <v>38933</v>
+        <v>38909</v>
       </c>
       <c r="K3" t="n">
-        <v>9414</v>
+        <v>9390</v>
       </c>
       <c r="L3" t="n">
-        <v>9907</v>
+        <v>9883</v>
       </c>
       <c r="M3" t="n">
-        <v>9794</v>
+        <v>9770</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -786,10 +747,10 @@
         </is>
       </c>
       <c r="O3" t="n">
-        <v>40699</v>
+        <v>40675</v>
       </c>
       <c r="P3" t="n">
-        <v>19811</v>
+        <v>19787</v>
       </c>
       <c r="Q3" t="n">
         <v>15336</v>
@@ -801,10 +762,10 @@
         <v>30309</v>
       </c>
       <c r="T3" t="n">
-        <v>26242</v>
+        <v>26218</v>
       </c>
       <c r="U3" t="n">
-        <v>8929</v>
+        <v>8905</v>
       </c>
       <c r="V3" t="inlineStr">
         <is>
@@ -813,7 +774,7 @@
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>Р</t>
+          <t>М</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
@@ -823,7 +784,7 @@
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>Р</t>
+          <t>М</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
@@ -863,7 +824,7 @@
       </c>
       <c r="AG3" t="inlineStr">
         <is>
-          <t>Р</t>
+          <t>ПР</t>
         </is>
       </c>
       <c r="AH3" t="inlineStr">
@@ -888,8 +849,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="n">
-        <v>44930</v>
+      <c r="A4" s="2" t="n">
+        <v>44929</v>
       </c>
       <c r="B4" t="n">
         <v>5</v>
@@ -905,25 +866,25 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>16473</v>
+        <v>33333</v>
       </c>
       <c r="H4" t="n">
-        <v>49879</v>
+        <v>49855</v>
       </c>
       <c r="I4" t="n">
         <v>34103</v>
       </c>
       <c r="J4" t="n">
-        <v>38957</v>
+        <v>38933</v>
       </c>
       <c r="K4" t="n">
-        <v>9438</v>
+        <v>9414</v>
       </c>
       <c r="L4" t="n">
-        <v>9931</v>
+        <v>9907</v>
       </c>
       <c r="M4" t="n">
-        <v>9818</v>
+        <v>9794</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -931,10 +892,10 @@
         </is>
       </c>
       <c r="O4" t="n">
-        <v>40723</v>
+        <v>40699</v>
       </c>
       <c r="P4" t="n">
-        <v>19835</v>
+        <v>19811</v>
       </c>
       <c r="Q4" t="n">
         <v>15336</v>
@@ -946,10 +907,10 @@
         <v>30309</v>
       </c>
       <c r="T4" t="n">
-        <v>26266</v>
+        <v>26242</v>
       </c>
       <c r="U4" t="n">
-        <v>8953</v>
+        <v>8929</v>
       </c>
       <c r="V4" t="inlineStr">
         <is>
@@ -1033,8 +994,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="n">
-        <v>44931</v>
+      <c r="A5" s="2" t="n">
+        <v>44930</v>
       </c>
       <c r="B5" t="n">
         <v>5</v>
@@ -1050,25 +1011,25 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>16473</v>
+        <v>444444</v>
       </c>
       <c r="H5" t="n">
-        <v>49903</v>
+        <v>49879</v>
       </c>
       <c r="I5" t="n">
         <v>34103</v>
       </c>
       <c r="J5" t="n">
-        <v>38981</v>
+        <v>38957</v>
       </c>
       <c r="K5" t="n">
-        <v>9462</v>
+        <v>9438</v>
       </c>
       <c r="L5" t="n">
-        <v>9955</v>
+        <v>9931</v>
       </c>
       <c r="M5" t="n">
-        <v>9842</v>
+        <v>9818</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -1076,13 +1037,13 @@
         </is>
       </c>
       <c r="O5" t="n">
-        <v>40747</v>
+        <v>40723</v>
       </c>
       <c r="P5" t="n">
-        <v>19859</v>
+        <v>19835</v>
       </c>
       <c r="Q5" t="n">
-        <v>15360</v>
+        <v>15336</v>
       </c>
       <c r="R5" t="n">
         <v>58529</v>
@@ -1094,7 +1055,7 @@
         <v>26266</v>
       </c>
       <c r="U5" t="n">
-        <v>8977</v>
+        <v>8953</v>
       </c>
       <c r="V5" t="inlineStr">
         <is>
@@ -1153,7 +1114,7 @@
       </c>
       <c r="AG5" t="inlineStr">
         <is>
-          <t>М</t>
+          <t>Р</t>
         </is>
       </c>
       <c r="AH5" t="inlineStr">
@@ -1168,7 +1129,7 @@
       </c>
       <c r="AJ5" t="inlineStr">
         <is>
-          <t>Р</t>
+          <t>М</t>
         </is>
       </c>
       <c r="AK5" t="inlineStr">
@@ -1178,8 +1139,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="n">
-        <v>44932</v>
+      <c r="A6" s="2" t="n">
+        <v>44931</v>
       </c>
       <c r="B6" t="n">
         <v>5</v>
@@ -1198,22 +1159,22 @@
         <v>16473</v>
       </c>
       <c r="H6" t="n">
-        <v>49927</v>
+        <v>49903</v>
       </c>
       <c r="I6" t="n">
         <v>34103</v>
       </c>
       <c r="J6" t="n">
-        <v>39005</v>
+        <v>38981</v>
       </c>
       <c r="K6" t="n">
-        <v>9486</v>
+        <v>9462</v>
       </c>
       <c r="L6" t="n">
-        <v>9979</v>
+        <v>9955</v>
       </c>
       <c r="M6" t="n">
-        <v>9866</v>
+        <v>9842</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -1221,13 +1182,13 @@
         </is>
       </c>
       <c r="O6" t="n">
-        <v>40771</v>
+        <v>40747</v>
       </c>
       <c r="P6" t="n">
-        <v>19883</v>
+        <v>19859</v>
       </c>
       <c r="Q6" t="n">
-        <v>15384</v>
+        <v>15360</v>
       </c>
       <c r="R6" t="n">
         <v>58529</v>
@@ -1239,7 +1200,7 @@
         <v>26266</v>
       </c>
       <c r="U6" t="n">
-        <v>9001</v>
+        <v>8977</v>
       </c>
       <c r="V6" t="inlineStr">
         <is>
@@ -1323,8 +1284,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="n">
-        <v>44933</v>
+      <c r="A7" s="2" t="n">
+        <v>44932</v>
       </c>
       <c r="B7" t="n">
         <v>5</v>
@@ -1343,22 +1304,22 @@
         <v>16473</v>
       </c>
       <c r="H7" t="n">
-        <v>49951</v>
+        <v>49927</v>
       </c>
       <c r="I7" t="n">
         <v>34103</v>
       </c>
       <c r="J7" t="n">
-        <v>39029</v>
+        <v>39005</v>
       </c>
       <c r="K7" t="n">
-        <v>9510</v>
+        <v>9486</v>
       </c>
       <c r="L7" t="n">
-        <v>10003</v>
+        <v>9979</v>
       </c>
       <c r="M7" t="n">
-        <v>9890</v>
+        <v>9866</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -1366,13 +1327,13 @@
         </is>
       </c>
       <c r="O7" t="n">
-        <v>40795</v>
+        <v>40771</v>
       </c>
       <c r="P7" t="n">
-        <v>19907</v>
+        <v>19883</v>
       </c>
       <c r="Q7" t="n">
-        <v>15408</v>
+        <v>15384</v>
       </c>
       <c r="R7" t="n">
         <v>58529</v>
@@ -1384,7 +1345,7 @@
         <v>26266</v>
       </c>
       <c r="U7" t="n">
-        <v>9025</v>
+        <v>9001</v>
       </c>
       <c r="V7" t="inlineStr">
         <is>
@@ -1403,7 +1364,7 @@
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>ПР</t>
+          <t>Р</t>
         </is>
       </c>
       <c r="Z7" t="inlineStr">
@@ -1468,8 +1429,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="n">
-        <v>44934</v>
+      <c r="A8" s="2" t="n">
+        <v>44933</v>
       </c>
       <c r="B8" t="n">
         <v>5</v>
@@ -1488,22 +1449,22 @@
         <v>16473</v>
       </c>
       <c r="H8" t="n">
-        <v>49975</v>
+        <v>49951</v>
       </c>
       <c r="I8" t="n">
         <v>34103</v>
       </c>
       <c r="J8" t="n">
-        <v>39053</v>
+        <v>39029</v>
       </c>
       <c r="K8" t="n">
-        <v>9534</v>
+        <v>9510</v>
       </c>
       <c r="L8" t="n">
-        <v>10027</v>
+        <v>10003</v>
       </c>
       <c r="M8" t="n">
-        <v>9914</v>
+        <v>9890</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -1511,13 +1472,13 @@
         </is>
       </c>
       <c r="O8" t="n">
-        <v>40819</v>
+        <v>40795</v>
       </c>
       <c r="P8" t="n">
-        <v>19931</v>
+        <v>19907</v>
       </c>
       <c r="Q8" t="n">
-        <v>15432</v>
+        <v>15408</v>
       </c>
       <c r="R8" t="n">
         <v>58529</v>
@@ -1529,7 +1490,7 @@
         <v>26266</v>
       </c>
       <c r="U8" t="n">
-        <v>9049</v>
+        <v>9025</v>
       </c>
       <c r="V8" t="inlineStr">
         <is>
@@ -1548,7 +1509,7 @@
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>Р</t>
+          <t>ПР</t>
         </is>
       </c>
       <c r="Z8" t="inlineStr">
@@ -1593,7 +1554,7 @@
       </c>
       <c r="AH8" t="inlineStr">
         <is>
-          <t>ПР</t>
+          <t>Р</t>
         </is>
       </c>
       <c r="AI8" t="inlineStr">
@@ -1613,8 +1574,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="n">
-        <v>44935</v>
+      <c r="A9" s="2" t="n">
+        <v>44934</v>
       </c>
       <c r="B9" t="n">
         <v>5</v>
@@ -1622,11 +1583,7 @@
       <c r="C9" t="n">
         <v>4</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>ОШ</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
@@ -1637,22 +1594,22 @@
         <v>16473</v>
       </c>
       <c r="H9" t="n">
-        <v>49991</v>
+        <v>49975</v>
       </c>
       <c r="I9" t="n">
         <v>34103</v>
       </c>
       <c r="J9" t="n">
-        <v>39077</v>
+        <v>39053</v>
       </c>
       <c r="K9" t="n">
-        <v>9550</v>
+        <v>9534</v>
       </c>
       <c r="L9" t="n">
-        <v>10051</v>
+        <v>10027</v>
       </c>
       <c r="M9" t="n">
-        <v>9938</v>
+        <v>9914</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1660,13 +1617,13 @@
         </is>
       </c>
       <c r="O9" t="n">
-        <v>40843</v>
+        <v>40819</v>
       </c>
       <c r="P9" t="n">
-        <v>19955</v>
+        <v>19931</v>
       </c>
       <c r="Q9" t="n">
-        <v>15456</v>
+        <v>15432</v>
       </c>
       <c r="R9" t="n">
         <v>58529</v>
@@ -1678,7 +1635,7 @@
         <v>26266</v>
       </c>
       <c r="U9" t="n">
-        <v>9073</v>
+        <v>9049</v>
       </c>
       <c r="V9" t="inlineStr">
         <is>
@@ -1692,7 +1649,7 @@
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>О</t>
+          <t>М</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
@@ -1707,7 +1664,7 @@
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>О</t>
+          <t>М</t>
         </is>
       </c>
       <c r="AB9" t="inlineStr">
@@ -1742,7 +1699,7 @@
       </c>
       <c r="AH9" t="inlineStr">
         <is>
-          <t>Р</t>
+          <t>ПР</t>
         </is>
       </c>
       <c r="AI9" t="inlineStr">
@@ -1762,8 +1719,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="n">
-        <v>44936</v>
+      <c r="A10" s="2" t="n">
+        <v>44935</v>
       </c>
       <c r="B10" t="n">
         <v>5</v>
@@ -1792,16 +1749,16 @@
         <v>34103</v>
       </c>
       <c r="J10" t="n">
-        <v>39101</v>
+        <v>39077</v>
       </c>
       <c r="K10" t="n">
-        <v>9574</v>
+        <v>9550</v>
       </c>
       <c r="L10" t="n">
-        <v>10075</v>
+        <v>10051</v>
       </c>
       <c r="M10" t="n">
-        <v>9962</v>
+        <v>9938</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1809,13 +1766,13 @@
         </is>
       </c>
       <c r="O10" t="n">
-        <v>40867</v>
+        <v>40843</v>
       </c>
       <c r="P10" t="n">
-        <v>19979</v>
+        <v>19955</v>
       </c>
       <c r="Q10" t="n">
-        <v>15480</v>
+        <v>15456</v>
       </c>
       <c r="R10" t="n">
         <v>58529</v>
@@ -1827,7 +1784,7 @@
         <v>26266</v>
       </c>
       <c r="U10" t="n">
-        <v>9097</v>
+        <v>9073</v>
       </c>
       <c r="V10" t="inlineStr">
         <is>
@@ -1841,7 +1798,7 @@
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>ГТД</t>
+          <t>О</t>
         </is>
       </c>
       <c r="Y10" t="inlineStr">
@@ -1856,7 +1813,7 @@
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>М</t>
+          <t>О</t>
         </is>
       </c>
       <c r="AB10" t="inlineStr">
@@ -1911,8 +1868,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="n">
-        <v>44937</v>
+      <c r="A11" s="2" t="n">
+        <v>44936</v>
       </c>
       <c r="B11" t="n">
         <v>5</v>
@@ -1941,16 +1898,16 @@
         <v>34103</v>
       </c>
       <c r="J11" t="n">
-        <v>39125</v>
+        <v>39101</v>
       </c>
       <c r="K11" t="n">
-        <v>9598</v>
+        <v>9574</v>
       </c>
       <c r="L11" t="n">
-        <v>10099</v>
+        <v>10075</v>
       </c>
       <c r="M11" t="n">
-        <v>9986</v>
+        <v>9962</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1958,13 +1915,13 @@
         </is>
       </c>
       <c r="O11" t="n">
-        <v>40891</v>
+        <v>40867</v>
       </c>
       <c r="P11" t="n">
-        <v>20003</v>
+        <v>19979</v>
       </c>
       <c r="Q11" t="n">
-        <v>15504</v>
+        <v>15480</v>
       </c>
       <c r="R11" t="n">
         <v>58529</v>
@@ -1976,7 +1933,7 @@
         <v>26266</v>
       </c>
       <c r="U11" t="n">
-        <v>9121</v>
+        <v>9097</v>
       </c>
       <c r="V11" t="inlineStr">
         <is>
@@ -2045,7 +2002,7 @@
       </c>
       <c r="AI11" t="inlineStr">
         <is>
-          <t>ПР</t>
+          <t>Р</t>
         </is>
       </c>
       <c r="AJ11" t="inlineStr">
@@ -2060,8 +2017,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="n">
-        <v>44938</v>
+      <c r="A12" s="2" t="n">
+        <v>44937</v>
       </c>
       <c r="B12" t="n">
         <v>5</v>
@@ -2090,16 +2047,16 @@
         <v>34103</v>
       </c>
       <c r="J12" t="n">
-        <v>39149</v>
+        <v>39125</v>
       </c>
       <c r="K12" t="n">
-        <v>9622</v>
+        <v>9598</v>
       </c>
       <c r="L12" t="n">
-        <v>10123</v>
+        <v>10099</v>
       </c>
       <c r="M12" t="n">
-        <v>10010</v>
+        <v>9986</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -2107,13 +2064,13 @@
         </is>
       </c>
       <c r="O12" t="n">
-        <v>40915</v>
+        <v>40891</v>
       </c>
       <c r="P12" t="n">
-        <v>20027</v>
+        <v>20003</v>
       </c>
       <c r="Q12" t="n">
-        <v>15528</v>
+        <v>15504</v>
       </c>
       <c r="R12" t="n">
         <v>58529</v>
@@ -2125,7 +2082,7 @@
         <v>26266</v>
       </c>
       <c r="U12" t="n">
-        <v>9145</v>
+        <v>9121</v>
       </c>
       <c r="V12" t="inlineStr">
         <is>
@@ -2194,7 +2151,7 @@
       </c>
       <c r="AI12" t="inlineStr">
         <is>
-          <t>Р</t>
+          <t>ПР</t>
         </is>
       </c>
       <c r="AJ12" t="inlineStr">
@@ -2209,8 +2166,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="n">
-        <v>44939</v>
+      <c r="A13" s="2" t="n">
+        <v>44938</v>
       </c>
       <c r="B13" t="n">
         <v>5</v>
@@ -2239,16 +2196,16 @@
         <v>34103</v>
       </c>
       <c r="J13" t="n">
-        <v>39173</v>
+        <v>39149</v>
       </c>
       <c r="K13" t="n">
-        <v>9646</v>
+        <v>9622</v>
       </c>
       <c r="L13" t="n">
-        <v>10147</v>
+        <v>10123</v>
       </c>
       <c r="M13" t="n">
-        <v>10034</v>
+        <v>10010</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
@@ -2256,13 +2213,13 @@
         </is>
       </c>
       <c r="O13" t="n">
-        <v>40939</v>
+        <v>40915</v>
       </c>
       <c r="P13" t="n">
-        <v>20051</v>
+        <v>20027</v>
       </c>
       <c r="Q13" t="n">
-        <v>15552</v>
+        <v>15528</v>
       </c>
       <c r="R13" t="n">
         <v>58529</v>
@@ -2274,84 +2231,233 @@
         <v>26266</v>
       </c>
       <c r="U13" t="n">
+        <v>9145</v>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>|</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>ГТД</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="AH13" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="AI13" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="AJ13" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="AK13" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>44939</v>
+      </c>
+      <c r="B14" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>4</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>ОШ</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>|</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>16473</v>
+      </c>
+      <c r="H14" t="n">
+        <v>49991</v>
+      </c>
+      <c r="I14" t="n">
+        <v>34103</v>
+      </c>
+      <c r="J14" t="n">
+        <v>39173</v>
+      </c>
+      <c r="K14" t="n">
+        <v>9646</v>
+      </c>
+      <c r="L14" t="n">
+        <v>10147</v>
+      </c>
+      <c r="M14" t="n">
+        <v>10034</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>|</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
+        <v>40939</v>
+      </c>
+      <c r="P14" t="n">
+        <v>20051</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>15552</v>
+      </c>
+      <c r="R14" t="n">
+        <v>58529</v>
+      </c>
+      <c r="S14" t="n">
+        <v>30309</v>
+      </c>
+      <c r="T14" t="n">
+        <v>26266</v>
+      </c>
+      <c r="U14" t="n">
         <v>9169</v>
       </c>
-      <c r="V13" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>Р</t>
-        </is>
-      </c>
-      <c r="X13" t="inlineStr">
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>|</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
         <is>
           <t>ГТД</t>
         </is>
       </c>
-      <c r="Y13" t="inlineStr">
-        <is>
-          <t>Р</t>
-        </is>
-      </c>
-      <c r="Z13" t="inlineStr">
-        <is>
-          <t>М</t>
-        </is>
-      </c>
-      <c r="AA13" t="inlineStr">
-        <is>
-          <t>М</t>
-        </is>
-      </c>
-      <c r="AB13" t="inlineStr">
-        <is>
-          <t>М</t>
-        </is>
-      </c>
-      <c r="AC13" t="inlineStr">
-        <is>
-          <t>М</t>
-        </is>
-      </c>
-      <c r="AD13" t="inlineStr">
-        <is>
-          <t>Р</t>
-        </is>
-      </c>
-      <c r="AE13" t="inlineStr">
-        <is>
-          <t>М</t>
-        </is>
-      </c>
-      <c r="AF13" t="inlineStr">
-        <is>
-          <t>М</t>
-        </is>
-      </c>
-      <c r="AG13" t="inlineStr">
-        <is>
-          <t>М</t>
-        </is>
-      </c>
-      <c r="AH13" t="inlineStr">
-        <is>
-          <t>Р</t>
-        </is>
-      </c>
-      <c r="AI13" t="inlineStr">
-        <is>
-          <t>Р</t>
-        </is>
-      </c>
-      <c r="AJ13" t="inlineStr">
-        <is>
-          <t>Р</t>
-        </is>
-      </c>
-      <c r="AK13" t="inlineStr">
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t>М</t>
+        </is>
+      </c>
+      <c r="AH14" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="AI14" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="AJ14" t="inlineStr">
+        <is>
+          <t>Р</t>
+        </is>
+      </c>
+      <c r="AK14" t="inlineStr">
         <is>
           <t>М</t>
         </is>

</xml_diff>